<commit_message>
Adds Create Game view
</commit_message>
<xml_diff>
--- a/StockMarketWebApp/backend/database/Database Design.xlsx
+++ b/StockMarketWebApp/backend/database/Database Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amygu\projects\Capstones\c-final-capstone-virtual-stock-market\StockMarketWebApp\backend\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39E5BE53-CCDA-4ECB-B59C-6D47A9E3BE8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8F93BA-0A34-488E-B892-EF3A8A787514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25530" yWindow="-2175" windowWidth="21600" windowHeight="11325" xr2:uid="{8049669E-021F-47C4-B34D-CAFD6E7D653A}"/>
+    <workbookView xWindow="1500" yWindow="264" windowWidth="21600" windowHeight="11328" xr2:uid="{8049669E-021F-47C4-B34D-CAFD6E7D653A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,18 +66,12 @@
     <t>creator_id (FK)</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>start_date</t>
   </si>
   <si>
     <t>end_date</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>user_id (FK, PK)</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>Dummy transaction for 0 shares to give them $100,000</t>
+  </si>
+  <si>
+    <t>game_desc</t>
+  </si>
+  <si>
+    <t>game_name</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,7 +527,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -535,13 +535,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -549,13 +549,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -563,13 +563,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -577,13 +577,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -591,10 +591,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -602,7 +602,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>